<commit_message>
removed alias column from 1_0_trimester_rep.xlsx
</commit_message>
<xml_diff>
--- a/dictionaries/chemicals/1_0/1_0_trimester_rep.xlsx
+++ b/dictionaries/chemicals/1_0/1_0_trimester_rep.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="101">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alias</t>
   </si>
   <si>
     <t xml:space="preserve">row_id</t>
@@ -996,13 +993,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:AMJ46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C1 A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="72.53"/>
@@ -1011,7 +1008,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1024,770 +1021,643 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B46" type="list">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B46" type="list">
       <formula1>"integer,decimal,text,binary,locale,boolean,datetime,date"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1802,11 +1672,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ171"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E:E C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="5" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="26"/>
@@ -1815,13 +1685,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
@@ -2340,8 +2210,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>